<commit_message>
Create problemformulering + product requirements
</commit_message>
<xml_diff>
--- a/Documents/PatientTaxi.xlsx
+++ b/Documents/PatientTaxi.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ejer\Documents\Github\Techcollege\Education\Module 6\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dani146d\Documents\GitHub\Techcollege\Education\Module 6\PatientTaxi\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E644F6C8-AB9C-4B92-A4D7-156522599228}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22754F63-DA8D-40FD-9828-B58A3066E5C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="1665" windowWidth="29040" windowHeight="15720" xr2:uid="{D5701FEF-667C-407A-91E1-C7B62C9D963E}"/>
+    <workbookView xWindow="-6945" yWindow="-21720" windowWidth="38640" windowHeight="21120" xr2:uid="{D5701FEF-667C-407A-91E1-C7B62C9D963E}"/>
   </bookViews>
   <sheets>
     <sheet name="Kravsspec" sheetId="3" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="61">
   <si>
     <t>Krav Id</t>
   </si>
@@ -74,14 +74,227 @@
     <t>Opfyldt</t>
   </si>
   <si>
-    <t>Brugeren bliver omstillet til loginsiden, hvis ingen login oplysninger er gemt</t>
+    <t>En bruger har en "Role" property, der bestemmer om brugeren er en sekretær/admin eller patient</t>
+  </si>
+  <si>
+    <t>Efter login skal brugeren viderestilels til /admin eller /patient alt efter rolle</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">På admin siden skal administratoren kunne udføre "CRUD" opreationer på </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Patient</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> modellen</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">På admin siden skal administratoren kunne udføre "CRUD" opreationer på </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Booking</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> modellen</t>
+    </r>
+  </si>
+  <si>
+    <t>En patient kan kun have 1 notat</t>
+  </si>
+  <si>
+    <t>En patient kan have flere bookings</t>
+  </si>
+  <si>
+    <t>På patientsiden kan patienten udføre CRUD operationer på deres egne bookings/bestillinger</t>
+  </si>
+  <si>
+    <t>Når en bestilling udføres, oprettes der forbindelse til en live-opdatering af taxaens estimerede tid</t>
+  </si>
+  <si>
+    <t>Patienten skal modtage en notifikation på hjemmesiden, når der er 1 time, 30 minutter, 20 minutter, 15 minutter, 10 minutter og 5 minutter tilbage til at taxaen er ankommet samt en notifikation, når taxaen er ankommet.</t>
+  </si>
+  <si>
+    <t>Brugere kan ikke udføre UPDATE eller DELETE operationer på booking, når der er en time tilbage til ankomsttid</t>
+  </si>
+  <si>
+    <t>På patientsiden kan patienten se deres eget notat</t>
+  </si>
+  <si>
+    <t>Brugernes kode skal enkrypteres før loginoplysningerne gemmes i databasen</t>
+  </si>
+  <si>
+    <t>Brugeren bliver omstillet til loginsiden</t>
+  </si>
+  <si>
+    <t>Efter brugerlogin gemmes en token i cookies, som er med til at verificere brugerens identitet</t>
+  </si>
+  <si>
+    <t>Omstilling til login</t>
+  </si>
+  <si>
+    <t>Usertoken</t>
+  </si>
+  <si>
+    <t>Role property</t>
+  </si>
+  <si>
+    <t>Viderestilling efter login</t>
+  </si>
+  <si>
+    <t>Admin CRUD Patient</t>
+  </si>
+  <si>
+    <t>Admin CRUD Notat</t>
+  </si>
+  <si>
+    <t>Admin CRUD Booking</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">På admin siden skal administratoren kunne udføre "CRUD" opreationer på </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Notat</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> modellen</t>
+    </r>
+  </si>
+  <si>
+    <t>Patient 1..1 Notat</t>
+  </si>
+  <si>
+    <t>Patient 1..* Booking</t>
+  </si>
+  <si>
+    <t>Patient R eget notat</t>
+  </si>
+  <si>
+    <t>Patient CRUD egen booking</t>
+  </si>
+  <si>
+    <t>Live opdatering efter bestilling</t>
+  </si>
+  <si>
+    <t>Notifikationsinterval</t>
+  </si>
+  <si>
+    <t>Ingen UD på Bookning en 1 time inden</t>
+  </si>
+  <si>
+    <t>Kodeordsenkryptering</t>
+  </si>
+  <si>
+    <t>Front1</t>
+  </si>
+  <si>
+    <t>Sikker1</t>
+  </si>
+  <si>
+    <t>Front2</t>
+  </si>
+  <si>
+    <t>Operation1</t>
+  </si>
+  <si>
+    <t>Operation2</t>
+  </si>
+  <si>
+    <t>Operation3</t>
+  </si>
+  <si>
+    <t>Operation4</t>
+  </si>
+  <si>
+    <t>Operation5</t>
+  </si>
+  <si>
+    <t>Front3</t>
+  </si>
+  <si>
+    <t>Front4</t>
+  </si>
+  <si>
+    <t>Operation6</t>
+  </si>
+  <si>
+    <t>Sikker2</t>
+  </si>
+  <si>
+    <t>Frontend</t>
+  </si>
+  <si>
+    <t>Entity</t>
+  </si>
+  <si>
+    <t>Entity1</t>
+  </si>
+  <si>
+    <t>Entity2</t>
+  </si>
+  <si>
+    <t>Entity3</t>
+  </si>
+  <si>
+    <t>Operation</t>
+  </si>
+  <si>
+    <t>Sikkerhed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -91,6 +304,14 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -455,216 +676,430 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{922BD6CB-9F3E-455F-858E-49A0A21094EE}">
-  <dimension ref="B2:G40"/>
+  <dimension ref="B2:G44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="7.7109375" customWidth="1"/>
-    <col min="3" max="3" width="23" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" customWidth="1"/>
-    <col min="5" max="6" width="8.85546875" customWidth="1"/>
-    <col min="7" max="7" width="183.28515625" customWidth="1"/>
+    <col min="3" max="3" width="14.44140625" customWidth="1"/>
+    <col min="4" max="4" width="34.109375" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" customWidth="1"/>
+    <col min="6" max="6" width="8.88671875" customWidth="1"/>
+    <col min="7" max="7" width="183.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="F2" s="3" t="s">
         <v>3</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>11</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B3" s="1"/>
+      <c r="C3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="G3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B4" s="1"/>
+      <c r="C4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" t="s">
+        <v>54</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B5" s="1"/>
+      <c r="C5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" t="s">
+        <v>55</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-    </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-    </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-    </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-    </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-    </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-    </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-    </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-    </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-    </row>
-    <row r="17" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-    </row>
-    <row r="18" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-    </row>
-    <row r="19" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-    </row>
-    <row r="20" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-    </row>
-    <row r="21" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E21" s="1"/>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B6" s="1"/>
+      <c r="C6" t="s">
+        <v>57</v>
+      </c>
+      <c r="D6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" t="s">
+        <v>55</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B7" s="1"/>
+      <c r="C7" t="s">
+        <v>58</v>
+      </c>
+      <c r="D7" t="s">
+        <v>35</v>
+      </c>
+      <c r="E7" t="s">
+        <v>55</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B8" s="1"/>
+      <c r="C8" t="s">
+        <v>45</v>
+      </c>
+      <c r="D8" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8" t="s">
+        <v>59</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B9" s="1"/>
+      <c r="C9" t="s">
+        <v>46</v>
+      </c>
+      <c r="D9" t="s">
+        <v>31</v>
+      </c>
+      <c r="E9" t="s">
+        <v>59</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B10" s="1"/>
+      <c r="C10" t="s">
+        <v>47</v>
+      </c>
+      <c r="D10" t="s">
+        <v>32</v>
+      </c>
+      <c r="E10" t="s">
+        <v>59</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B11" s="1"/>
+      <c r="C11" t="s">
+        <v>43</v>
+      </c>
+      <c r="D11" t="s">
+        <v>41</v>
+      </c>
+      <c r="E11" t="s">
+        <v>60</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B12" s="1"/>
+      <c r="C12" t="s">
+        <v>48</v>
+      </c>
+      <c r="D12" t="s">
+        <v>36</v>
+      </c>
+      <c r="E12" t="s">
+        <v>59</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B13" s="1"/>
+      <c r="C13" t="s">
+        <v>49</v>
+      </c>
+      <c r="D13" t="s">
+        <v>37</v>
+      </c>
+      <c r="E13" t="s">
+        <v>59</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B14" s="1"/>
+      <c r="C14" t="s">
+        <v>52</v>
+      </c>
+      <c r="D14" t="s">
+        <v>40</v>
+      </c>
+      <c r="E14" t="s">
+        <v>59</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B15" s="1"/>
+      <c r="C15" t="s">
+        <v>50</v>
+      </c>
+      <c r="D15" t="s">
+        <v>38</v>
+      </c>
+      <c r="E15" t="s">
+        <v>54</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B16" s="1"/>
+      <c r="C16" t="s">
+        <v>51</v>
+      </c>
+      <c r="D16" t="s">
+        <v>39</v>
+      </c>
+      <c r="E16" t="s">
+        <v>54</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G16" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B17" s="1"/>
+      <c r="C17" t="s">
+        <v>53</v>
+      </c>
+      <c r="D17" t="s">
+        <v>27</v>
+      </c>
+      <c r="E17" t="s">
+        <v>60</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G17" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B21" s="1"/>
       <c r="F21" s="1"/>
     </row>
-    <row r="22" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E22" s="1"/>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B22" s="1"/>
       <c r="F22" s="1"/>
     </row>
-    <row r="23" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E23" s="1"/>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B23" s="1"/>
       <c r="F23" s="1"/>
     </row>
-    <row r="24" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E24" s="1"/>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B24" s="1"/>
       <c r="F24" s="1"/>
     </row>
-    <row r="25" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E25" s="1"/>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B25" s="1"/>
       <c r="F25" s="1"/>
     </row>
-    <row r="26" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E26" s="1"/>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B26" s="1"/>
       <c r="F26" s="1"/>
     </row>
-    <row r="27" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E27" s="1"/>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B27" s="1"/>
       <c r="F27" s="1"/>
     </row>
-    <row r="28" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E28" s="1"/>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B28" s="1"/>
       <c r="F28" s="1"/>
     </row>
-    <row r="29" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E29" s="1"/>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B29" s="1"/>
       <c r="F29" s="1"/>
     </row>
-    <row r="30" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E30" s="1"/>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B30" s="1"/>
       <c r="F30" s="1"/>
     </row>
-    <row r="31" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E31" s="1"/>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B31" s="1"/>
       <c r="F31" s="1"/>
     </row>
-    <row r="32" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E32" s="1"/>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B32" s="1"/>
       <c r="F32" s="1"/>
     </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C35" t="s">
+    <row r="33" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B33" s="1"/>
+      <c r="F33" s="1"/>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B34" s="1"/>
+      <c r="F34" s="1"/>
+    </row>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B35" s="1"/>
+      <c r="F35" s="1"/>
+    </row>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B36" s="1"/>
+      <c r="F36" s="1"/>
+    </row>
+    <row r="39" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="D39" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B36">
+    <row r="40" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C40">
         <v>5</v>
       </c>
-      <c r="C36" t="s">
+      <c r="D40" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B37">
+    <row r="41" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C41">
         <v>4</v>
       </c>
-      <c r="C37" t="s">
+      <c r="D41" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B38">
+    <row r="42" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C42">
         <v>3</v>
       </c>
-      <c r="C38" t="s">
+      <c r="D42" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B39">
+    <row r="43" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C43">
         <v>2</v>
       </c>
-      <c r="C39" t="s">
+      <c r="D43" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B40">
+    <row r="44" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C44">
         <v>1</v>
       </c>
-      <c r="C40" t="s">
+      <c r="D44" t="s">
         <v>9</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C3:G20">
+    <sortCondition ref="F3:F20" customList="Skal,Burde,Kunne,Gerne"/>
+  </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E32" xr:uid="{FDF4FD2E-07EE-4D02-97CE-EC8E16AA54D8}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F17 F21:F36" xr:uid="{FDF4FD2E-07EE-4D02-97CE-EC8E16AA54D8}">
       <formula1>"Skal,Burde,Kunne,Gerne,Hvis tid"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F32" xr:uid="{74B0885D-C444-4534-93C9-A891D8F15A37}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:B17 B21:B36" xr:uid="{74B0885D-C444-4534-93C9-A891D8F15A37}">
       <formula1>"Ja,Nej,Delvist"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>